<commit_message>
Removed logic for range prediction
</commit_message>
<xml_diff>
--- a/input/Pune Real Estate Data.xlsx
+++ b/input/Pune Real Estate Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sudhanshu\gitrepository\Data-Science-Projects\Real-Estate-Price-Prediction-Model-with-NLP-and-FastAPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sudhanshu\gitrepository\Data-Science-Projects\End-to-End-Real-Estate-Price-Prediction-Model\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF95F0A1-7B94-401D-9D7A-3896E90D50CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4A955B-5BED-42C3-9AB2-4067D289C8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2636" uniqueCount="401">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -1650,7 +1650,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1738,10 +1738,9 @@
         <v>492</v>
       </c>
       <c r="F2" s="1">
-        <v>39</v>
+        <v>3900000</v>
       </c>
       <c r="G2" s="1">
-        <f>F2*0.1</f>
         <v>3.9000000000000004</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1795,10 +1794,9 @@
         <v>774</v>
       </c>
       <c r="F3" s="1">
-        <v>65</v>
+        <v>6500000</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G66" si="0">F3*0.1</f>
         <v>6.5</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1852,10 +1850,9 @@
         <v>889</v>
       </c>
       <c r="F4" s="1">
-        <v>74</v>
+        <v>7400000</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
         <v>7.4</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1909,10 +1906,9 @@
         <v>1018</v>
       </c>
       <c r="F5" s="1">
-        <v>89</v>
+        <v>8900000</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
         <v>8.9</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1966,10 +1962,9 @@
         <v>743</v>
       </c>
       <c r="F6" s="1">
-        <v>74</v>
+        <v>7400000</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="0"/>
         <v>7.4</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -2023,10 +2018,9 @@
         <v>975</v>
       </c>
       <c r="F7" s="1">
-        <v>95</v>
+        <v>9500000</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -2080,10 +2074,9 @@
         <v>28</v>
       </c>
       <c r="F8" s="1">
-        <v>75</v>
+        <v>7500000</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -2137,10 +2130,9 @@
         <v>29</v>
       </c>
       <c r="F9" s="1">
-        <v>100</v>
+        <v>10000000</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -2194,10 +2186,9 @@
         <v>905</v>
       </c>
       <c r="F10" s="1">
-        <v>65</v>
+        <v>6500000</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -2251,10 +2242,9 @@
         <v>1125</v>
       </c>
       <c r="F11" s="1">
-        <v>88</v>
+        <v>8800000</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="0"/>
         <v>8.8000000000000007</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -2308,10 +2298,9 @@
         <v>1644</v>
       </c>
       <c r="F12" s="1">
-        <v>135</v>
+        <v>13500000</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -2365,10 +2354,9 @@
         <v>2220</v>
       </c>
       <c r="F13" s="1">
-        <v>188</v>
+        <v>18800000</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="0"/>
         <v>18.8</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -2422,10 +2410,9 @@
         <v>2220</v>
       </c>
       <c r="F14" s="1">
-        <v>188</v>
+        <v>18800000</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="0"/>
         <v>18.8</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -2479,10 +2466,9 @@
         <v>41</v>
       </c>
       <c r="F15" s="1">
-        <v>58</v>
+        <v>5800000</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="0"/>
         <v>5.8000000000000007</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -2536,10 +2522,9 @@
         <v>42</v>
       </c>
       <c r="F16" s="1">
-        <v>95</v>
+        <v>9500000</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -2593,10 +2578,9 @@
         <v>423</v>
       </c>
       <c r="F17" s="1">
-        <v>40</v>
+        <v>4000000</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -2650,10 +2634,9 @@
         <v>665</v>
       </c>
       <c r="F18" s="1">
-        <v>58</v>
+        <v>5800000</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="0"/>
         <v>5.8000000000000007</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -2707,10 +2690,9 @@
         <v>45</v>
       </c>
       <c r="F19" s="1">
-        <v>78</v>
+        <v>7800000</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="0"/>
         <v>7.8000000000000007</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -2764,10 +2746,9 @@
         <v>462</v>
       </c>
       <c r="F20" s="1">
-        <v>36</v>
+        <v>3600000</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -2821,10 +2802,9 @@
         <v>666</v>
       </c>
       <c r="F21" s="1">
-        <v>48</v>
+        <v>4800000</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="0"/>
         <v>4.8000000000000007</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -2878,10 +2858,9 @@
         <v>750</v>
       </c>
       <c r="F22" s="1">
-        <v>57</v>
+        <v>5700000</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="0"/>
         <v>5.7</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -2935,10 +2914,9 @@
         <v>1030</v>
       </c>
       <c r="F23" s="1">
-        <v>79</v>
+        <v>7900000</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="0"/>
         <v>7.9</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -2992,10 +2970,9 @@
         <v>446</v>
       </c>
       <c r="F24" s="1">
-        <v>37</v>
+        <v>3700000</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="0"/>
         <v>3.7</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -3049,10 +3026,9 @@
         <v>796</v>
       </c>
       <c r="F25" s="1">
-        <v>57</v>
+        <v>5700000</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="0"/>
         <v>5.7</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -3106,10 +3082,9 @@
         <v>842</v>
       </c>
       <c r="F26" s="1">
-        <v>59</v>
+        <v>5900000</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="0"/>
         <v>5.9</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -3163,10 +3138,9 @@
         <v>865</v>
       </c>
       <c r="F27" s="1">
-        <v>61</v>
+        <v>6100000</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="0"/>
         <v>6.1000000000000005</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -3220,10 +3194,9 @@
         <v>902</v>
       </c>
       <c r="F28" s="1">
-        <v>63</v>
+        <v>6300000</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="0"/>
         <v>6.3000000000000007</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -3277,10 +3250,9 @@
         <v>1154</v>
       </c>
       <c r="F29" s="1">
-        <v>79</v>
+        <v>7900000</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="0"/>
         <v>7.9</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -3334,10 +3306,9 @@
         <v>872</v>
       </c>
       <c r="F30" s="1">
-        <v>61</v>
+        <v>6100000</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="0"/>
         <v>6.1000000000000005</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -3391,10 +3362,9 @@
         <v>934</v>
       </c>
       <c r="F31" s="1">
-        <v>65</v>
+        <v>6500000</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -3448,10 +3418,9 @@
         <v>1088</v>
       </c>
       <c r="F32" s="1">
-        <v>73</v>
+        <v>7300000</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="0"/>
         <v>7.3000000000000007</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -3505,10 +3474,9 @@
         <v>1109</v>
       </c>
       <c r="F33" s="1">
-        <v>76</v>
+        <v>7600000</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="0"/>
         <v>7.6000000000000005</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -3562,10 +3530,9 @@
         <v>1163</v>
       </c>
       <c r="F34" s="1">
-        <v>80</v>
+        <v>8000000</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -3619,10 +3586,9 @@
         <v>1419</v>
       </c>
       <c r="F35" s="1">
-        <v>96</v>
+        <v>9600000</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="0"/>
         <v>9.6000000000000014</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -3676,10 +3642,9 @@
         <v>1485</v>
       </c>
       <c r="F36" s="1">
-        <v>100</v>
+        <v>10000000</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -3733,10 +3698,9 @@
         <v>684</v>
       </c>
       <c r="F37" s="1">
-        <v>70</v>
+        <v>7000000</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -3790,10 +3754,9 @@
         <v>990</v>
       </c>
       <c r="F38" s="1">
-        <v>90</v>
+        <v>9000000</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -3847,10 +3810,9 @@
         <v>882</v>
       </c>
       <c r="F39" s="1">
-        <v>97</v>
+        <v>9700000</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="0"/>
         <v>9.7000000000000011</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -3904,10 +3866,9 @@
         <v>1103</v>
       </c>
       <c r="F40" s="1">
-        <v>120</v>
+        <v>12000000</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -3961,10 +3922,9 @@
         <v>543</v>
       </c>
       <c r="F41" s="1">
-        <v>42</v>
+        <v>4200000</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -4015,10 +3975,9 @@
         <v>59</v>
       </c>
       <c r="F42" s="1">
-        <v>57</v>
+        <v>5700000</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" si="0"/>
         <v>5.7</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -4071,9 +4030,8 @@
       <c r="F43" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G43" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="G43" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>51</v>
@@ -4123,10 +4081,9 @@
         <v>320</v>
       </c>
       <c r="F44" s="1">
-        <v>14</v>
+        <v>1400000</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" si="0"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="H44" s="1" t="s">
@@ -4177,10 +4134,9 @@
         <v>473</v>
       </c>
       <c r="F45" s="1">
-        <v>22</v>
+        <v>2200000</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="H45" s="1" t="s">
@@ -4231,10 +4187,9 @@
         <v>581</v>
       </c>
       <c r="F46" s="1">
-        <v>26</v>
+        <v>2600000</v>
       </c>
       <c r="G46" s="1">
-        <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
       <c r="H46" s="1" t="s">
@@ -4285,10 +4240,9 @@
         <v>790</v>
       </c>
       <c r="F47" s="1">
-        <v>80</v>
+        <v>8000000</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H47" s="1" t="s">
@@ -4342,10 +4296,9 @@
         <v>820</v>
       </c>
       <c r="F48" s="1">
-        <v>83</v>
+        <v>8300000</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" si="0"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="H48" s="1" t="s">
@@ -4399,10 +4352,9 @@
         <v>989</v>
       </c>
       <c r="F49" s="1">
-        <v>101</v>
+        <v>10100000</v>
       </c>
       <c r="G49" s="1">
-        <f t="shared" si="0"/>
         <v>10.100000000000001</v>
       </c>
       <c r="H49" s="1" t="s">
@@ -4456,10 +4408,9 @@
         <v>1003</v>
       </c>
       <c r="F50" s="1">
-        <v>103</v>
+        <v>10300000</v>
       </c>
       <c r="G50" s="1">
-        <f t="shared" si="0"/>
         <v>10.3</v>
       </c>
       <c r="H50" s="1" t="s">
@@ -4513,10 +4464,9 @@
         <v>1182</v>
       </c>
       <c r="F51" s="1">
-        <v>128</v>
+        <v>12800000</v>
       </c>
       <c r="G51" s="1">
-        <f t="shared" si="0"/>
         <v>12.8</v>
       </c>
       <c r="H51" s="1" t="s">
@@ -4570,10 +4520,9 @@
         <v>1579</v>
       </c>
       <c r="F52" s="1">
-        <v>163</v>
+        <v>16300000</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="0"/>
         <v>16.3</v>
       </c>
       <c r="H52" s="1" t="s">
@@ -4627,10 +4576,9 @@
         <v>163</v>
       </c>
       <c r="F53" s="1">
-        <v>54</v>
+        <v>5400000</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -4681,10 +4629,9 @@
         <v>491</v>
       </c>
       <c r="F54" s="1">
-        <v>39</v>
+        <v>3900000</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="0"/>
         <v>3.9000000000000004</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -4735,10 +4682,9 @@
         <v>659</v>
       </c>
       <c r="F55" s="1">
-        <v>51</v>
+        <v>5100000</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" si="0"/>
         <v>5.1000000000000005</v>
       </c>
       <c r="H55" s="1" t="s">
@@ -4789,10 +4735,9 @@
         <v>732</v>
       </c>
       <c r="F56" s="1">
-        <v>60</v>
+        <v>6000000</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H56" s="1" t="s">
@@ -4843,10 +4788,9 @@
         <v>809</v>
       </c>
       <c r="F57" s="1">
-        <v>66</v>
+        <v>6600000</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="0"/>
         <v>6.6000000000000005</v>
       </c>
       <c r="H57" s="1" t="s">
@@ -4897,10 +4841,9 @@
         <v>460</v>
       </c>
       <c r="F58" s="1">
-        <v>45.5</v>
+        <v>4550000</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" si="0"/>
         <v>4.55</v>
       </c>
       <c r="H58" s="1" t="s">
@@ -4951,10 +4894,9 @@
         <v>734</v>
       </c>
       <c r="F59" s="1">
-        <v>72.5</v>
+        <v>7250000</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="0"/>
         <v>7.25</v>
       </c>
       <c r="H59" s="1" t="s">
@@ -5005,10 +4947,9 @@
         <v>753</v>
       </c>
       <c r="F60" s="1">
-        <v>73.5</v>
+        <v>7350000</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" si="0"/>
         <v>7.3500000000000005</v>
       </c>
       <c r="H60" s="1" t="s">
@@ -5059,10 +5000,9 @@
         <v>675</v>
       </c>
       <c r="F61" s="1">
-        <v>62</v>
+        <v>6200000</v>
       </c>
       <c r="G61" s="1">
-        <f t="shared" si="0"/>
         <v>6.2</v>
       </c>
       <c r="H61" s="1" t="s">
@@ -5113,10 +5053,9 @@
         <v>917</v>
       </c>
       <c r="F62" s="1">
-        <v>84</v>
+        <v>8400000</v>
       </c>
       <c r="G62" s="1">
-        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
       <c r="H62" s="1" t="s">
@@ -5167,10 +5106,9 @@
         <v>670</v>
       </c>
       <c r="F63" s="1">
-        <v>54.14</v>
+        <v>5414000</v>
       </c>
       <c r="G63" s="1">
-        <f t="shared" si="0"/>
         <v>5.4140000000000006</v>
       </c>
       <c r="H63" s="1" t="s">
@@ -5221,10 +5159,9 @@
         <v>740</v>
       </c>
       <c r="F64" s="1">
-        <v>58.32</v>
+        <v>5832000</v>
       </c>
       <c r="G64" s="1">
-        <f t="shared" si="0"/>
         <v>5.8320000000000007</v>
       </c>
       <c r="H64" s="1" t="s">
@@ -5275,10 +5212,9 @@
         <v>847</v>
       </c>
       <c r="F65" s="1">
-        <v>69.38</v>
+        <v>6938000</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" si="0"/>
         <v>6.9379999999999997</v>
       </c>
       <c r="H65" s="1" t="s">
@@ -5329,10 +5265,9 @@
         <v>936</v>
       </c>
       <c r="F66" s="1">
-        <v>75.03</v>
+        <v>7503000</v>
       </c>
       <c r="G66" s="1">
-        <f t="shared" si="0"/>
         <v>7.5030000000000001</v>
       </c>
       <c r="H66" s="1" t="s">
@@ -5383,10 +5318,9 @@
         <v>990</v>
       </c>
       <c r="F67" s="1">
-        <v>79.02</v>
+        <v>7902000</v>
       </c>
       <c r="G67" s="1">
-        <f t="shared" ref="G67:G130" si="1">F67*0.1</f>
         <v>7.9020000000000001</v>
       </c>
       <c r="H67" s="1" t="s">
@@ -5437,10 +5371,9 @@
         <v>1032</v>
       </c>
       <c r="F68" s="1">
-        <v>82.1</v>
+        <v>8209999.9999999991</v>
       </c>
       <c r="G68" s="1">
-        <f t="shared" si="1"/>
         <v>8.2099999999999991</v>
       </c>
       <c r="H68" s="1" t="s">
@@ -5491,10 +5424,9 @@
         <v>1698</v>
       </c>
       <c r="F69" s="1">
-        <v>249</v>
+        <v>24900000</v>
       </c>
       <c r="G69" s="1">
-        <f t="shared" si="1"/>
         <v>24.900000000000002</v>
       </c>
       <c r="H69" s="1" t="s">
@@ -5545,10 +5477,9 @@
         <v>2267</v>
       </c>
       <c r="F70" s="1">
-        <v>460</v>
+        <v>46000000</v>
       </c>
       <c r="G70" s="1">
-        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="H70" s="1" t="s">
@@ -5600,10 +5531,9 @@
         <v>670</v>
       </c>
       <c r="F71" s="1">
-        <v>45.75</v>
+        <v>4575000</v>
       </c>
       <c r="G71" s="1">
-        <f t="shared" si="1"/>
         <v>4.5750000000000002</v>
       </c>
       <c r="H71" s="1" t="s">
@@ -5654,10 +5584,9 @@
         <v>725</v>
       </c>
       <c r="F72" s="1">
-        <v>49.34</v>
+        <v>4934000</v>
       </c>
       <c r="G72" s="1">
-        <f t="shared" si="1"/>
         <v>4.9340000000000011</v>
       </c>
       <c r="H72" s="1" t="s">
@@ -5708,10 +5637,9 @@
         <v>731</v>
       </c>
       <c r="F73" s="1">
-        <v>49.74</v>
+        <v>4974000</v>
       </c>
       <c r="G73" s="1">
-        <f t="shared" si="1"/>
         <v>4.9740000000000002</v>
       </c>
       <c r="H73" s="1" t="s">
@@ -5762,10 +5690,9 @@
         <v>744</v>
       </c>
       <c r="F74" s="1">
-        <v>50.56</v>
+        <v>5056000</v>
       </c>
       <c r="G74" s="1">
-        <f t="shared" si="1"/>
         <v>5.0560000000000009</v>
       </c>
       <c r="H74" s="1" t="s">
@@ -5816,10 +5743,9 @@
         <v>923</v>
       </c>
       <c r="F75" s="1">
-        <v>923</v>
+        <v>92300000</v>
       </c>
       <c r="G75" s="1">
-        <f t="shared" si="1"/>
         <v>92.300000000000011</v>
       </c>
       <c r="H75" s="1" t="s">
@@ -5870,10 +5796,9 @@
         <v>930</v>
       </c>
       <c r="F76" s="1">
-        <v>930</v>
+        <v>93000000</v>
       </c>
       <c r="G76" s="1">
-        <f t="shared" si="1"/>
         <v>93</v>
       </c>
       <c r="H76" s="1" t="s">
@@ -5924,10 +5849,9 @@
         <v>446</v>
       </c>
       <c r="F77" s="1">
-        <v>36</v>
+        <v>3600000</v>
       </c>
       <c r="G77" s="1">
-        <f t="shared" si="1"/>
         <v>3.6</v>
       </c>
       <c r="H77" s="1" t="s">
@@ -5978,10 +5902,9 @@
         <v>670</v>
       </c>
       <c r="F78" s="1">
-        <v>55</v>
+        <v>5500000</v>
       </c>
       <c r="G78" s="1">
-        <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
       <c r="H78" s="1" t="s">
@@ -6032,10 +5955,9 @@
         <v>792</v>
       </c>
       <c r="F79" s="1">
-        <v>65.5</v>
+        <v>6550000</v>
       </c>
       <c r="G79" s="1">
-        <f t="shared" si="1"/>
         <v>6.5500000000000007</v>
       </c>
       <c r="H79" s="1" t="s">
@@ -6086,10 +6008,9 @@
         <v>1180</v>
       </c>
       <c r="F80" s="1">
-        <v>68</v>
+        <v>6800000</v>
       </c>
       <c r="G80" s="1">
-        <f t="shared" si="1"/>
         <v>6.8000000000000007</v>
       </c>
       <c r="H80" s="1" t="s">
@@ -6140,10 +6061,9 @@
         <v>860</v>
       </c>
       <c r="F81" s="1">
-        <v>65</v>
+        <v>6500000</v>
       </c>
       <c r="G81" s="1">
-        <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
       <c r="H81" s="1" t="s">
@@ -6194,10 +6114,9 @@
         <v>988</v>
       </c>
       <c r="F82" s="1">
-        <v>92</v>
+        <v>9200000</v>
       </c>
       <c r="G82" s="1">
-        <f t="shared" si="1"/>
         <v>9.2000000000000011</v>
       </c>
       <c r="H82" s="1" t="s">
@@ -6248,10 +6167,9 @@
         <v>1093</v>
       </c>
       <c r="F83" s="1">
-        <v>92</v>
+        <v>9200000</v>
       </c>
       <c r="G83" s="1">
-        <f t="shared" si="1"/>
         <v>9.2000000000000011</v>
       </c>
       <c r="H83" s="1" t="s">
@@ -6302,10 +6220,9 @@
         <v>456</v>
       </c>
       <c r="F84" s="1">
-        <v>33.5</v>
+        <v>3350000</v>
       </c>
       <c r="G84" s="1">
-        <f t="shared" si="1"/>
         <v>3.35</v>
       </c>
       <c r="H84" s="1" t="s">
@@ -6356,10 +6273,9 @@
         <v>644</v>
       </c>
       <c r="F85" s="1">
-        <v>47.3</v>
+        <v>4730000</v>
       </c>
       <c r="G85" s="1">
-        <f t="shared" si="1"/>
         <v>4.7299999999999995</v>
       </c>
       <c r="H85" s="1" t="s">
@@ -6410,10 +6326,9 @@
         <v>785</v>
       </c>
       <c r="F86" s="1">
-        <v>55.22</v>
+        <v>5522000</v>
       </c>
       <c r="G86" s="1">
-        <f t="shared" si="1"/>
         <v>5.5220000000000002</v>
       </c>
       <c r="H86" s="1" t="s">
@@ -6464,10 +6379,9 @@
         <v>1060</v>
       </c>
       <c r="F87" s="1">
-        <v>136</v>
+        <v>13600000</v>
       </c>
       <c r="G87" s="1">
-        <f t="shared" si="1"/>
         <v>13.600000000000001</v>
       </c>
       <c r="H87" s="1" t="s">
@@ -6518,10 +6432,9 @@
         <v>113</v>
       </c>
       <c r="F88" s="1">
-        <v>143</v>
+        <v>14300000</v>
       </c>
       <c r="G88" s="1">
-        <f t="shared" si="1"/>
         <v>14.3</v>
       </c>
       <c r="H88" s="1" t="s">
@@ -6572,10 +6485,9 @@
         <v>664</v>
       </c>
       <c r="F89" s="1">
-        <v>47.59</v>
+        <v>4759000</v>
       </c>
       <c r="G89" s="1">
-        <f t="shared" si="1"/>
         <v>4.7590000000000003</v>
       </c>
       <c r="H89" s="1" t="s">
@@ -6626,10 +6538,9 @@
         <v>670</v>
       </c>
       <c r="F90" s="1">
-        <v>47.7</v>
+        <v>4770000</v>
       </c>
       <c r="G90" s="1">
-        <f t="shared" si="1"/>
         <v>4.7700000000000005</v>
       </c>
       <c r="H90" s="1" t="s">
@@ -6680,10 +6591,9 @@
         <v>673</v>
       </c>
       <c r="F91" s="1">
-        <v>47.8</v>
+        <v>4780000</v>
       </c>
       <c r="G91" s="1">
-        <f t="shared" si="1"/>
         <v>4.78</v>
       </c>
       <c r="H91" s="1" t="s">
@@ -6734,10 +6644,9 @@
         <v>682</v>
       </c>
       <c r="F92" s="1">
-        <v>47.91</v>
+        <v>4791000</v>
       </c>
       <c r="G92" s="1">
-        <f t="shared" si="1"/>
         <v>4.7909999999999995</v>
       </c>
       <c r="H92" s="1" t="s">
@@ -6788,10 +6697,9 @@
         <v>698</v>
       </c>
       <c r="F93" s="1">
-        <v>48.02</v>
+        <v>4802000</v>
       </c>
       <c r="G93" s="1">
-        <f t="shared" si="1"/>
         <v>4.8020000000000005</v>
       </c>
       <c r="H93" s="1" t="s">
@@ -6842,10 +6750,9 @@
         <v>1239</v>
       </c>
       <c r="F94" s="1">
-        <v>161</v>
+        <v>16100000</v>
       </c>
       <c r="G94" s="1">
-        <f t="shared" si="1"/>
         <v>16.100000000000001</v>
       </c>
       <c r="H94" s="1" t="s">
@@ -6896,10 +6803,9 @@
         <v>1315</v>
       </c>
       <c r="F95" s="1">
-        <v>170</v>
+        <v>17000000</v>
       </c>
       <c r="G95" s="1">
-        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="H95" s="1" t="s">
@@ -6950,10 +6856,9 @@
         <v>1388</v>
       </c>
       <c r="F96" s="1">
-        <v>178</v>
+        <v>17800000</v>
       </c>
       <c r="G96" s="1">
-        <f t="shared" si="1"/>
         <v>17.8</v>
       </c>
       <c r="H96" s="1" t="s">
@@ -7004,10 +6909,9 @@
         <v>1463</v>
       </c>
       <c r="F97" s="1">
-        <v>187</v>
+        <v>18700000</v>
       </c>
       <c r="G97" s="1">
-        <f t="shared" si="1"/>
         <v>18.7</v>
       </c>
       <c r="H97" s="1" t="s">
@@ -7058,10 +6962,9 @@
         <v>1671</v>
       </c>
       <c r="F98" s="1">
-        <v>211</v>
+        <v>21100000</v>
       </c>
       <c r="G98" s="1">
-        <f t="shared" si="1"/>
         <v>21.1</v>
       </c>
       <c r="H98" s="1" t="s">
@@ -7112,10 +7015,9 @@
         <v>1687</v>
       </c>
       <c r="F99" s="1">
-        <v>213</v>
+        <v>21300000</v>
       </c>
       <c r="G99" s="1">
-        <f t="shared" si="1"/>
         <v>21.3</v>
       </c>
       <c r="H99" s="1" t="s">
@@ -7166,10 +7068,9 @@
         <v>575</v>
       </c>
       <c r="F100" s="1">
-        <v>65</v>
+        <v>6500000</v>
       </c>
       <c r="G100" s="1">
-        <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
       <c r="H100" s="1" t="s">
@@ -7220,10 +7121,9 @@
         <v>751</v>
       </c>
       <c r="F101" s="1">
-        <v>84</v>
+        <v>8400000</v>
       </c>
       <c r="G101" s="1">
-        <f t="shared" si="1"/>
         <v>8.4</v>
       </c>
       <c r="H101" s="1" t="s">
@@ -7274,10 +7174,9 @@
         <v>761</v>
       </c>
       <c r="F102" s="1">
-        <v>85</v>
+        <v>8500000</v>
       </c>
       <c r="G102" s="1">
-        <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
       <c r="H102" s="1" t="s">
@@ -7328,10 +7227,9 @@
         <v>871</v>
       </c>
       <c r="F103" s="1">
-        <v>96</v>
+        <v>9600000</v>
       </c>
       <c r="G103" s="1">
-        <f t="shared" si="1"/>
         <v>9.6000000000000014</v>
       </c>
       <c r="H103" s="1" t="s">
@@ -7382,10 +7280,9 @@
         <v>1166</v>
       </c>
       <c r="F104" s="1">
-        <v>129</v>
+        <v>12900000</v>
       </c>
       <c r="G104" s="1">
-        <f t="shared" si="1"/>
         <v>12.9</v>
       </c>
       <c r="H104" s="1" t="s">
@@ -7436,10 +7333,9 @@
         <v>1206</v>
       </c>
       <c r="F105" s="1">
-        <v>133</v>
+        <v>13300000</v>
       </c>
       <c r="G105" s="1">
-        <f t="shared" si="1"/>
         <v>13.3</v>
       </c>
       <c r="H105" s="1" t="s">
@@ -7490,10 +7386,9 @@
         <v>1272</v>
       </c>
       <c r="F106" s="1">
-        <v>139</v>
+        <v>13900000</v>
       </c>
       <c r="G106" s="1">
-        <f t="shared" si="1"/>
         <v>13.9</v>
       </c>
       <c r="H106" s="1" t="s">
@@ -7544,10 +7439,9 @@
         <v>1279</v>
       </c>
       <c r="F107" s="1">
-        <v>140</v>
+        <v>14000000</v>
       </c>
       <c r="G107" s="1">
-        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="H107" s="1" t="s">
@@ -7598,10 +7492,9 @@
         <v>646</v>
       </c>
       <c r="F108" s="1">
-        <v>43.2</v>
+        <v>4320000</v>
       </c>
       <c r="G108" s="1">
-        <f t="shared" si="1"/>
         <v>4.32</v>
       </c>
       <c r="H108" s="1" t="s">
@@ -7652,10 +7545,9 @@
         <v>717</v>
       </c>
       <c r="F109" s="1">
-        <v>47.4</v>
+        <v>4740000</v>
       </c>
       <c r="G109" s="1">
-        <f t="shared" si="1"/>
         <v>4.74</v>
       </c>
       <c r="H109" s="1" t="s">
@@ -7706,10 +7598,9 @@
         <v>436</v>
       </c>
       <c r="F110" s="1">
-        <v>30.58</v>
+        <v>3058000</v>
       </c>
       <c r="G110" s="1">
-        <f t="shared" si="1"/>
         <v>3.0579999999999998</v>
       </c>
       <c r="H110" s="1" t="s">
@@ -7760,10 +7651,9 @@
         <v>637</v>
       </c>
       <c r="F111" s="1">
-        <v>43.49</v>
+        <v>4349000</v>
       </c>
       <c r="G111" s="1">
-        <f t="shared" si="1"/>
         <v>4.3490000000000002</v>
       </c>
       <c r="H111" s="1" t="s">
@@ -7814,10 +7704,9 @@
         <v>642</v>
       </c>
       <c r="F112" s="1">
-        <v>43.83</v>
+        <v>4383000</v>
       </c>
       <c r="G112" s="1">
-        <f t="shared" si="1"/>
         <v>4.383</v>
       </c>
       <c r="H112" s="1" t="s">
@@ -7868,10 +7757,9 @@
         <v>655</v>
       </c>
       <c r="F113" s="1">
-        <v>44.44</v>
+        <v>4444000</v>
       </c>
       <c r="G113" s="1">
-        <f t="shared" si="1"/>
         <v>4.444</v>
       </c>
       <c r="H113" s="1" t="s">
@@ -7922,10 +7810,9 @@
         <v>668</v>
       </c>
       <c r="F114" s="1">
-        <v>45.52</v>
+        <v>4552000</v>
       </c>
       <c r="G114" s="1">
-        <f t="shared" si="1"/>
         <v>4.5520000000000005</v>
       </c>
       <c r="H114" s="1" t="s">
@@ -7976,10 +7863,9 @@
         <v>810</v>
       </c>
       <c r="F115" s="1">
-        <v>54</v>
+        <v>5400000</v>
       </c>
       <c r="G115" s="1">
-        <f t="shared" si="1"/>
         <v>5.4</v>
       </c>
       <c r="H115" s="1" t="s">
@@ -8030,10 +7916,9 @@
         <v>735</v>
       </c>
       <c r="F116" s="1">
-        <v>111</v>
+        <v>11100000</v>
       </c>
       <c r="G116" s="1">
-        <f t="shared" si="1"/>
         <v>11.100000000000001</v>
       </c>
       <c r="H116" s="1" t="s">
@@ -8084,10 +7969,9 @@
         <v>783</v>
       </c>
       <c r="F117" s="1">
-        <v>118</v>
+        <v>11800000</v>
       </c>
       <c r="G117" s="1">
-        <f t="shared" si="1"/>
         <v>11.8</v>
       </c>
       <c r="H117" s="1" t="s">
@@ -8138,10 +8022,9 @@
         <v>805</v>
       </c>
       <c r="F118" s="1">
-        <v>121</v>
+        <v>12100000</v>
       </c>
       <c r="G118" s="1">
-        <f t="shared" si="1"/>
         <v>12.100000000000001</v>
       </c>
       <c r="H118" s="1" t="s">
@@ -8192,10 +8075,9 @@
         <v>1074</v>
       </c>
       <c r="F119" s="1">
-        <v>162</v>
+        <v>16200000</v>
       </c>
       <c r="G119" s="1">
-        <f t="shared" si="1"/>
         <v>16.2</v>
       </c>
       <c r="H119" s="1" t="s">
@@ -8246,10 +8128,9 @@
         <v>1111</v>
       </c>
       <c r="F120" s="1">
-        <v>167</v>
+        <v>16700000</v>
       </c>
       <c r="G120" s="1">
-        <f t="shared" si="1"/>
         <v>16.7</v>
       </c>
       <c r="H120" s="1" t="s">
@@ -8300,10 +8181,9 @@
         <v>535</v>
       </c>
       <c r="F121" s="1">
-        <v>36</v>
+        <v>3600000</v>
       </c>
       <c r="G121" s="1">
-        <f t="shared" si="1"/>
         <v>3.6</v>
       </c>
       <c r="H121" s="1" t="s">
@@ -8354,10 +8234,9 @@
         <v>725</v>
       </c>
       <c r="F122" s="1">
-        <v>52</v>
+        <v>5200000</v>
       </c>
       <c r="G122" s="1">
-        <f t="shared" si="1"/>
         <v>5.2</v>
       </c>
       <c r="H122" s="1" t="s">
@@ -8408,10 +8287,9 @@
         <v>810</v>
       </c>
       <c r="F123" s="1">
-        <v>79</v>
+        <v>7900000</v>
       </c>
       <c r="G123" s="1">
-        <f t="shared" si="1"/>
         <v>7.9</v>
       </c>
       <c r="H123" s="1" t="s">
@@ -8462,10 +8340,9 @@
         <v>947</v>
       </c>
       <c r="F124" s="1">
-        <v>97</v>
+        <v>9700000</v>
       </c>
       <c r="G124" s="1">
-        <f t="shared" si="1"/>
         <v>9.7000000000000011</v>
       </c>
       <c r="H124" s="1" t="s">
@@ -8516,10 +8393,9 @@
         <v>697</v>
       </c>
       <c r="F125" s="1">
-        <v>68.06</v>
+        <v>6806000</v>
       </c>
       <c r="G125" s="1">
-        <f t="shared" si="1"/>
         <v>6.8060000000000009</v>
       </c>
       <c r="H125" s="1" t="s">
@@ -8570,10 +8446,9 @@
         <v>711</v>
       </c>
       <c r="F126" s="1">
-        <v>68.41</v>
+        <v>6841000</v>
       </c>
       <c r="G126" s="1">
-        <f t="shared" si="1"/>
         <v>6.8410000000000002</v>
       </c>
       <c r="H126" s="1" t="s">
@@ -8624,10 +8499,9 @@
         <v>792</v>
       </c>
       <c r="F127" s="1">
-        <v>78</v>
+        <v>7800000</v>
       </c>
       <c r="G127" s="1">
-        <f t="shared" si="1"/>
         <v>7.8000000000000007</v>
       </c>
       <c r="H127" s="1" t="s">
@@ -8678,10 +8552,9 @@
         <v>980</v>
       </c>
       <c r="F128" s="1">
-        <v>98.87</v>
+        <v>9887000</v>
       </c>
       <c r="G128" s="1">
-        <f t="shared" si="1"/>
         <v>9.8870000000000005</v>
       </c>
       <c r="H128" s="1" t="s">
@@ -8732,10 +8605,9 @@
         <v>1400</v>
       </c>
       <c r="F129" s="1">
-        <v>140</v>
+        <v>14000000</v>
       </c>
       <c r="G129" s="1">
-        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="H129" s="1" t="s">
@@ -8786,10 +8658,9 @@
         <v>1772</v>
       </c>
       <c r="F130" s="1">
-        <v>177</v>
+        <v>17700000</v>
       </c>
       <c r="G130" s="1">
-        <f t="shared" si="1"/>
         <v>17.7</v>
       </c>
       <c r="H130" s="1" t="s">
@@ -8840,10 +8711,9 @@
         <v>732</v>
       </c>
       <c r="F131" s="1">
-        <v>68.8</v>
+        <v>6880000</v>
       </c>
       <c r="G131" s="1">
-        <f t="shared" ref="G131:G194" si="2">F131*0.1</f>
         <v>6.88</v>
       </c>
       <c r="H131" s="1" t="s">
@@ -8894,10 +8764,9 @@
         <v>751</v>
       </c>
       <c r="F132" s="1">
-        <v>68.8</v>
+        <v>6880000</v>
       </c>
       <c r="G132" s="1">
-        <f t="shared" si="2"/>
         <v>6.88</v>
       </c>
       <c r="H132" s="1" t="s">
@@ -8948,10 +8817,9 @@
         <v>1662</v>
       </c>
       <c r="F133" s="1">
-        <v>130</v>
+        <v>13000000</v>
       </c>
       <c r="G133" s="1">
-        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="H133" s="1" t="s">
@@ -9002,10 +8870,9 @@
         <v>705</v>
       </c>
       <c r="F134" s="1">
-        <v>48</v>
+        <v>4800000</v>
       </c>
       <c r="G134" s="1">
-        <f t="shared" si="2"/>
         <v>4.8000000000000007</v>
       </c>
       <c r="H134" s="1" t="s">
@@ -9056,10 +8923,9 @@
         <v>726</v>
       </c>
       <c r="F135" s="1">
-        <v>51</v>
+        <v>5100000</v>
       </c>
       <c r="G135" s="1">
-        <f t="shared" si="2"/>
         <v>5.1000000000000005</v>
       </c>
       <c r="H135" s="1" t="s">
@@ -9110,10 +8976,9 @@
         <v>809</v>
       </c>
       <c r="F136" s="1">
-        <v>56</v>
+        <v>5600000</v>
       </c>
       <c r="G136" s="1">
-        <f t="shared" si="2"/>
         <v>5.6000000000000005</v>
       </c>
       <c r="H136" s="1" t="s">
@@ -9164,10 +9029,9 @@
         <v>734</v>
       </c>
       <c r="F137" s="1">
-        <v>95</v>
+        <v>9500000</v>
       </c>
       <c r="G137" s="1">
-        <f t="shared" si="2"/>
         <v>9.5</v>
       </c>
       <c r="H137" s="1" t="s">
@@ -9218,10 +9082,9 @@
         <v>793</v>
       </c>
       <c r="F138" s="1">
-        <v>110</v>
+        <v>11000000</v>
       </c>
       <c r="G138" s="1">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="H138" s="1" t="s">
@@ -9272,10 +9135,9 @@
         <v>904</v>
       </c>
       <c r="F139" s="1">
-        <v>118</v>
+        <v>11800000</v>
       </c>
       <c r="G139" s="1">
-        <f t="shared" si="2"/>
         <v>11.8</v>
       </c>
       <c r="H139" s="1" t="s">
@@ -9326,10 +9188,9 @@
         <v>1154</v>
       </c>
       <c r="F140" s="1">
-        <v>146</v>
+        <v>14600000</v>
       </c>
       <c r="G140" s="1">
-        <f t="shared" si="2"/>
         <v>14.600000000000001</v>
       </c>
       <c r="H140" s="1" t="s">
@@ -9380,10 +9241,9 @@
         <v>1168</v>
       </c>
       <c r="F141" s="1">
-        <v>147</v>
+        <v>14700000</v>
       </c>
       <c r="G141" s="1">
-        <f t="shared" si="2"/>
         <v>14.700000000000001</v>
       </c>
       <c r="H141" s="1" t="s">
@@ -9434,10 +9294,9 @@
         <v>1189</v>
       </c>
       <c r="F142" s="1">
-        <v>149</v>
+        <v>14900000</v>
       </c>
       <c r="G142" s="1">
-        <f t="shared" si="2"/>
         <v>14.9</v>
       </c>
       <c r="H142" s="1" t="s">
@@ -9488,10 +9347,9 @@
         <v>479</v>
       </c>
       <c r="F143" s="1">
-        <v>38.68</v>
+        <v>3868000</v>
       </c>
       <c r="G143" s="1">
-        <f t="shared" si="2"/>
         <v>3.8680000000000003</v>
       </c>
       <c r="H143" s="1" t="s">
@@ -9542,10 +9400,9 @@
         <v>693</v>
       </c>
       <c r="F144" s="1">
-        <v>58</v>
+        <v>5800000</v>
       </c>
       <c r="G144" s="1">
-        <f t="shared" si="2"/>
         <v>5.8000000000000007</v>
       </c>
       <c r="H144" s="1" t="s">
@@ -9596,10 +9453,9 @@
         <v>725</v>
       </c>
       <c r="F145" s="1">
-        <v>60.72</v>
+        <v>6072000</v>
       </c>
       <c r="G145" s="1">
-        <f t="shared" si="2"/>
         <v>6.0720000000000001</v>
       </c>
       <c r="H145" s="1" t="s">
@@ -9650,10 +9506,9 @@
         <v>808</v>
       </c>
       <c r="F146" s="1">
-        <v>81.489999999999995</v>
+        <v>8148999.9999999991</v>
       </c>
       <c r="G146" s="1">
-        <f t="shared" si="2"/>
         <v>8.1489999999999991</v>
       </c>
       <c r="H146" s="1" t="s">
@@ -9704,10 +9559,9 @@
         <v>1086</v>
       </c>
       <c r="F147" s="1">
-        <v>108</v>
+        <v>10800000</v>
       </c>
       <c r="G147" s="1">
-        <f t="shared" si="2"/>
         <v>10.8</v>
       </c>
       <c r="H147" s="1" t="s">
@@ -9758,10 +9612,9 @@
         <v>785</v>
       </c>
       <c r="F148" s="1">
-        <v>74.5</v>
+        <v>7450000</v>
       </c>
       <c r="G148" s="1">
-        <f t="shared" si="2"/>
         <v>7.45</v>
       </c>
       <c r="H148" s="1" t="s">
@@ -9812,10 +9665,9 @@
         <v>844</v>
       </c>
       <c r="F149" s="1">
-        <v>80.59</v>
+        <v>8059000</v>
       </c>
       <c r="G149" s="1">
-        <f t="shared" si="2"/>
         <v>8.0590000000000011</v>
       </c>
       <c r="H149" s="1" t="s">
@@ -9866,10 +9718,9 @@
         <v>873</v>
       </c>
       <c r="F150" s="1">
-        <v>83</v>
+        <v>8300000</v>
       </c>
       <c r="G150" s="1">
-        <f t="shared" si="2"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="H150" s="1" t="s">
@@ -9920,10 +9771,9 @@
         <v>606</v>
       </c>
       <c r="F151" s="1">
-        <v>47.25</v>
+        <v>4725000</v>
       </c>
       <c r="G151" s="1">
-        <f t="shared" si="2"/>
         <v>4.7250000000000005</v>
       </c>
       <c r="H151" s="1" t="s">
@@ -9974,10 +9824,9 @@
         <v>611</v>
       </c>
       <c r="F152" s="1">
-        <v>47.5</v>
+        <v>4750000</v>
       </c>
       <c r="G152" s="1">
-        <f t="shared" si="2"/>
         <v>4.75</v>
       </c>
       <c r="H152" s="1" t="s">
@@ -10028,10 +9877,9 @@
         <v>626</v>
       </c>
       <c r="F153" s="1">
-        <v>48.43</v>
+        <v>4843000</v>
       </c>
       <c r="G153" s="1">
-        <f t="shared" si="2"/>
         <v>4.843</v>
       </c>
       <c r="H153" s="1" t="s">
@@ -10082,10 +9930,9 @@
         <v>691</v>
       </c>
       <c r="F154" s="1">
-        <v>55.26</v>
+        <v>5526000</v>
       </c>
       <c r="G154" s="1">
-        <f t="shared" si="2"/>
         <v>5.5259999999999998</v>
       </c>
       <c r="H154" s="1" t="s">
@@ -10136,10 +9983,9 @@
         <v>835</v>
       </c>
       <c r="F155" s="1">
-        <v>66</v>
+        <v>6600000</v>
       </c>
       <c r="G155" s="1">
-        <f t="shared" si="2"/>
         <v>6.6000000000000005</v>
       </c>
       <c r="H155" s="1" t="s">
@@ -10190,10 +10036,9 @@
         <v>854</v>
       </c>
       <c r="F156" s="1">
-        <v>67</v>
+        <v>6700000</v>
       </c>
       <c r="G156" s="1">
-        <f t="shared" si="2"/>
         <v>6.7</v>
       </c>
       <c r="H156" s="1" t="s">
@@ -10244,10 +10089,9 @@
         <v>626</v>
       </c>
       <c r="F157" s="1">
-        <v>45.7</v>
+        <v>4570000</v>
       </c>
       <c r="G157" s="1">
-        <f t="shared" si="2"/>
         <v>4.57</v>
       </c>
       <c r="H157" s="1" t="s">
@@ -10298,10 +10142,9 @@
         <v>715</v>
       </c>
       <c r="F158" s="1">
-        <v>45.5</v>
+        <v>4550000</v>
       </c>
       <c r="G158" s="1">
-        <f t="shared" si="2"/>
         <v>4.55</v>
       </c>
       <c r="H158" s="1" t="s">
@@ -10352,10 +10195,9 @@
         <v>159</v>
       </c>
       <c r="F159" s="1">
-        <v>59</v>
+        <v>5900000</v>
       </c>
       <c r="G159" s="1">
-        <f t="shared" si="2"/>
         <v>5.9</v>
       </c>
       <c r="H159" s="1" t="s">
@@ -10406,10 +10248,9 @@
         <v>968</v>
       </c>
       <c r="F160" s="1">
-        <v>87</v>
+        <v>8700000</v>
       </c>
       <c r="G160" s="1">
-        <f t="shared" si="2"/>
         <v>8.7000000000000011</v>
       </c>
       <c r="H160" s="1" t="s">
@@ -10460,10 +10301,9 @@
         <v>996</v>
       </c>
       <c r="F161" s="1">
-        <v>89</v>
+        <v>8900000</v>
       </c>
       <c r="G161" s="1">
-        <f t="shared" si="2"/>
         <v>8.9</v>
       </c>
       <c r="H161" s="1" t="s">
@@ -10514,10 +10354,9 @@
         <v>1038</v>
       </c>
       <c r="F162" s="1">
-        <v>92</v>
+        <v>9200000</v>
       </c>
       <c r="G162" s="1">
-        <f t="shared" si="2"/>
         <v>9.2000000000000011</v>
       </c>
       <c r="H162" s="1" t="s">
@@ -10568,10 +10407,9 @@
         <v>489</v>
       </c>
       <c r="F163" s="1">
-        <v>43.8</v>
+        <v>4380000</v>
       </c>
       <c r="G163" s="1">
-        <f t="shared" si="2"/>
         <v>4.38</v>
       </c>
       <c r="H163" s="1" t="s">
@@ -10622,10 +10460,9 @@
         <v>598</v>
       </c>
       <c r="F164" s="1">
-        <v>55.3</v>
+        <v>5530000</v>
       </c>
       <c r="G164" s="1">
-        <f t="shared" si="2"/>
         <v>5.53</v>
       </c>
       <c r="H164" s="1" t="s">
@@ -10676,10 +10513,9 @@
         <v>616</v>
       </c>
       <c r="F165" s="1">
-        <v>56.5</v>
+        <v>5650000</v>
       </c>
       <c r="G165" s="1">
-        <f t="shared" si="2"/>
         <v>5.65</v>
       </c>
       <c r="H165" s="1" t="s">
@@ -10730,10 +10566,9 @@
         <v>692</v>
       </c>
       <c r="F166" s="1">
-        <v>62.3</v>
+        <v>6230000</v>
       </c>
       <c r="G166" s="1">
-        <f t="shared" si="2"/>
         <v>6.23</v>
       </c>
       <c r="H166" s="1" t="s">
@@ -10784,10 +10619,9 @@
         <v>867</v>
       </c>
       <c r="F167" s="1">
-        <v>79.3</v>
+        <v>7930000</v>
       </c>
       <c r="G167" s="1">
-        <f t="shared" si="2"/>
         <v>7.93</v>
       </c>
       <c r="H167" s="1" t="s">
@@ -10838,10 +10672,9 @@
         <v>908</v>
       </c>
       <c r="F168" s="1">
-        <v>82.5</v>
+        <v>8250000</v>
       </c>
       <c r="G168" s="1">
-        <f t="shared" si="2"/>
         <v>8.25</v>
       </c>
       <c r="H168" s="1" t="s">
@@ -10892,10 +10725,9 @@
         <v>1624</v>
       </c>
       <c r="F169" s="1">
-        <v>159</v>
+        <v>15900000</v>
       </c>
       <c r="G169" s="1">
-        <f t="shared" si="2"/>
         <v>15.9</v>
       </c>
       <c r="H169" s="1" t="s">
@@ -10946,10 +10778,9 @@
         <v>2043</v>
       </c>
       <c r="F170" s="1">
-        <v>215</v>
+        <v>21500000</v>
       </c>
       <c r="G170" s="1">
-        <f t="shared" si="2"/>
         <v>21.5</v>
       </c>
       <c r="H170" s="1" t="s">
@@ -11000,10 +10831,9 @@
         <v>727</v>
       </c>
       <c r="F171" s="1">
-        <v>45.74</v>
+        <v>4574000</v>
       </c>
       <c r="G171" s="1">
-        <f t="shared" si="2"/>
         <v>4.5740000000000007</v>
       </c>
       <c r="H171" s="1" t="s">
@@ -11054,10 +10884,9 @@
         <v>923</v>
       </c>
       <c r="F172" s="1">
-        <v>58.95</v>
+        <v>5895000</v>
       </c>
       <c r="G172" s="1">
-        <f t="shared" si="2"/>
         <v>5.8950000000000005</v>
       </c>
       <c r="H172" s="1" t="s">
@@ -11108,10 +10937,9 @@
         <v>171</v>
       </c>
       <c r="F173" s="1">
-        <v>59</v>
+        <v>5900000</v>
       </c>
       <c r="G173" s="1">
-        <f t="shared" si="2"/>
         <v>5.9</v>
       </c>
       <c r="H173" s="1" t="s">
@@ -11162,10 +10990,9 @@
         <v>170</v>
       </c>
       <c r="F174" s="1">
-        <v>109</v>
+        <v>10900000</v>
       </c>
       <c r="G174" s="1">
-        <f t="shared" si="2"/>
         <v>10.9</v>
       </c>
       <c r="H174" s="1" t="s">
@@ -11216,10 +11043,9 @@
         <v>408</v>
       </c>
       <c r="F175" s="1">
-        <v>39.99</v>
+        <v>3999000</v>
       </c>
       <c r="G175" s="1">
-        <f t="shared" si="2"/>
         <v>3.9990000000000006</v>
       </c>
       <c r="H175" s="1" t="s">
@@ -11270,10 +11096,9 @@
         <v>546</v>
       </c>
       <c r="F176" s="1">
-        <v>53.99</v>
+        <v>5399000</v>
       </c>
       <c r="G176" s="1">
-        <f t="shared" si="2"/>
         <v>5.3990000000000009</v>
       </c>
       <c r="H176" s="1" t="s">
@@ -11324,10 +11149,9 @@
         <v>629</v>
       </c>
       <c r="F177" s="1">
-        <v>59.99</v>
+        <v>5999000</v>
       </c>
       <c r="G177" s="1">
-        <f t="shared" si="2"/>
         <v>5.9990000000000006</v>
       </c>
       <c r="H177" s="1" t="s">
@@ -11378,10 +11202,9 @@
         <v>378</v>
       </c>
       <c r="F178" s="1">
-        <v>33</v>
+        <v>3300000</v>
       </c>
       <c r="G178" s="1">
-        <f t="shared" si="2"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="H178" s="1" t="s">
@@ -11432,10 +11255,9 @@
         <v>494</v>
       </c>
       <c r="F179" s="1">
-        <v>47</v>
+        <v>4700000</v>
       </c>
       <c r="G179" s="1">
-        <f t="shared" si="2"/>
         <v>4.7</v>
       </c>
       <c r="H179" s="1" t="s">
@@ -11486,10 +11308,9 @@
         <v>780</v>
       </c>
       <c r="F180" s="1">
-        <v>70</v>
+        <v>7000000</v>
       </c>
       <c r="G180" s="1">
-        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="H180" s="1" t="s">
@@ -11540,10 +11361,9 @@
         <v>850</v>
       </c>
       <c r="F181" s="1">
-        <v>73</v>
+        <v>7300000</v>
       </c>
       <c r="G181" s="1">
-        <f t="shared" si="2"/>
         <v>7.3000000000000007</v>
       </c>
       <c r="H181" s="1" t="s">
@@ -11594,10 +11414,9 @@
         <v>900</v>
       </c>
       <c r="F182" s="1">
-        <v>78</v>
+        <v>7800000</v>
       </c>
       <c r="G182" s="1">
-        <f t="shared" si="2"/>
         <v>7.8000000000000007</v>
       </c>
       <c r="H182" s="1" t="s">
@@ -11648,10 +11467,9 @@
         <v>930</v>
       </c>
       <c r="F183" s="1">
-        <v>83</v>
+        <v>8300000</v>
       </c>
       <c r="G183" s="1">
-        <f t="shared" si="2"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="H183" s="1" t="s">
@@ -11702,10 +11520,9 @@
         <v>179</v>
       </c>
       <c r="F184" s="1">
-        <v>175</v>
+        <v>17500000</v>
       </c>
       <c r="G184" s="1">
-        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="H184" s="1" t="s">
@@ -11756,10 +11573,9 @@
         <v>1740</v>
       </c>
       <c r="F185" s="1">
-        <v>250</v>
+        <v>25000000</v>
       </c>
       <c r="G185" s="1">
-        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="H185" s="1" t="s">
@@ -11810,10 +11626,9 @@
         <v>2447</v>
       </c>
       <c r="F186" s="1">
-        <v>420</v>
+        <v>42000000</v>
       </c>
       <c r="G186" s="1">
-        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="H186" s="1" t="s">
@@ -11864,10 +11679,9 @@
         <v>405</v>
       </c>
       <c r="F187" s="1">
-        <v>39.49</v>
+        <v>3949000</v>
       </c>
       <c r="G187" s="1">
-        <f t="shared" si="2"/>
         <v>3.9490000000000003</v>
       </c>
       <c r="H187" s="1" t="s">
@@ -11918,10 +11732,9 @@
         <v>408</v>
       </c>
       <c r="F188" s="1">
-        <v>39.49</v>
+        <v>3949000</v>
       </c>
       <c r="G188" s="1">
-        <f t="shared" si="2"/>
         <v>3.9490000000000003</v>
       </c>
       <c r="H188" s="1" t="s">
@@ -11972,10 +11785,9 @@
         <v>392</v>
       </c>
       <c r="F189" s="1">
-        <v>39.49</v>
+        <v>3949000</v>
       </c>
       <c r="G189" s="1">
-        <f t="shared" si="2"/>
         <v>3.9490000000000003</v>
       </c>
       <c r="H189" s="1" t="s">
@@ -12026,10 +11838,9 @@
         <v>667</v>
       </c>
       <c r="F190" s="1">
-        <v>64.989999999999995</v>
+        <v>6498999.9999999991</v>
       </c>
       <c r="G190" s="1">
-        <f t="shared" si="2"/>
         <v>6.4989999999999997</v>
       </c>
       <c r="H190" s="1" t="s">
@@ -12080,10 +11891,9 @@
         <v>641</v>
       </c>
       <c r="F191" s="1">
-        <v>64.989999999999995</v>
+        <v>6498999.9999999991</v>
       </c>
       <c r="G191" s="1">
-        <f t="shared" si="2"/>
         <v>6.4989999999999997</v>
       </c>
       <c r="H191" s="1" t="s">
@@ -12134,10 +11944,9 @@
         <v>665</v>
       </c>
       <c r="F192" s="1">
-        <v>64.989999999999995</v>
+        <v>6498999.9999999991</v>
       </c>
       <c r="G192" s="1">
-        <f t="shared" si="2"/>
         <v>6.4989999999999997</v>
       </c>
       <c r="H192" s="1" t="s">
@@ -12188,10 +11997,9 @@
         <v>280</v>
       </c>
       <c r="F193" s="1">
-        <v>13.19</v>
+        <v>1319000</v>
       </c>
       <c r="G193" s="1">
-        <f t="shared" si="2"/>
         <v>1.319</v>
       </c>
       <c r="H193" s="1" t="s">
@@ -12242,10 +12050,9 @@
         <v>385</v>
       </c>
       <c r="F194" s="1">
-        <v>17.29</v>
+        <v>1729000</v>
       </c>
       <c r="G194" s="1">
-        <f t="shared" si="2"/>
         <v>1.7290000000000001</v>
       </c>
       <c r="H194" s="1" t="s">
@@ -12296,10 +12103,9 @@
         <v>730</v>
       </c>
       <c r="F195" s="1">
-        <v>87</v>
+        <v>8700000</v>
       </c>
       <c r="G195" s="1">
-        <f t="shared" ref="G195:G201" si="3">F195*0.1</f>
         <v>8.7000000000000011</v>
       </c>
       <c r="H195" s="1" t="s">
@@ -12353,10 +12159,9 @@
         <v>189</v>
       </c>
       <c r="F196" s="1">
-        <v>129</v>
+        <v>12900000</v>
       </c>
       <c r="G196" s="1">
-        <f t="shared" si="3"/>
         <v>12.9</v>
       </c>
       <c r="H196" s="1" t="s">
@@ -12410,10 +12215,9 @@
         <v>190</v>
       </c>
       <c r="F197" s="1">
-        <v>160</v>
+        <v>16000000</v>
       </c>
       <c r="G197" s="1">
-        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="H197" s="1" t="s">
@@ -12467,10 +12271,9 @@
         <v>191</v>
       </c>
       <c r="F198" s="1">
-        <v>230</v>
+        <v>23000000</v>
       </c>
       <c r="G198" s="1">
-        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="H198" s="1" t="s">
@@ -12524,10 +12327,9 @@
         <v>194</v>
       </c>
       <c r="F199" s="1">
-        <v>95</v>
+        <v>9500000</v>
       </c>
       <c r="G199" s="1">
-        <f t="shared" si="3"/>
         <v>9.5</v>
       </c>
       <c r="H199" s="1" t="s">
@@ -12581,10 +12383,9 @@
         <v>197</v>
       </c>
       <c r="F200" s="1">
-        <v>135</v>
+        <v>13500000</v>
       </c>
       <c r="G200" s="1">
-        <f t="shared" si="3"/>
         <v>13.5</v>
       </c>
       <c r="H200" s="1" t="s">
@@ -12638,10 +12439,9 @@
         <v>776</v>
       </c>
       <c r="F201" s="1">
-        <v>90.68</v>
+        <v>9068000</v>
       </c>
       <c r="G201" s="1">
-        <f t="shared" si="3"/>
         <v>9.0680000000000014</v>
       </c>
       <c r="H201" s="1" t="s">

</xml_diff>